<commit_message>
excel zrihtu da ohranja stile in za brisanje inputov prikaz
</commit_message>
<xml_diff>
--- a/desktop-app/electron-app/public/bonitetna-ocena-template.xlsx
+++ b/desktop-app/electron-app/public/bonitetna-ocena-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Domen\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Domen\Desktop\IPT 2\PRAKTIKUM 2\PRII\desktop-app\electron-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22D304E-C528-4601-ABA4-74E314477891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16957564-2224-4883-BCD1-C89B9911541A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5776,8 +5776,8 @@
   </sheetPr>
   <dimension ref="A1:J133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6051,15 +6051,9 @@
     <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="18"/>
       <c r="B24" s="21"/>
-      <c r="C24" s="55">
-        <v>45323</v>
-      </c>
-      <c r="D24" s="55">
-        <v>45352</v>
-      </c>
-      <c r="E24" s="55">
-        <v>45383</v>
-      </c>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
       <c r="F24" s="18"/>
     </row>
     <row r="25" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>